<commit_message>
Added more Metadata-driven tabs
</commit_message>
<xml_diff>
--- a/DataContract_AdventureWorksSQL.XLSX
+++ b/DataContract_AdventureWorksSQL.XLSX
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aanelson\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\DataContracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86772CEF-B9D2-435C-8351-B8C1D10D1D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5179FC5B-D69C-4018-BD4C-906FC64C7EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66570" yWindow="5385" windowWidth="20295" windowHeight="15105" xr2:uid="{C220A797-1A06-4A38-BB9F-5D87810F53A4}"/>
+    <workbookView xWindow="64260" yWindow="1380" windowWidth="20295" windowHeight="15105" xr2:uid="{C220A797-1A06-4A38-BB9F-5D87810F53A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Connection" sheetId="2" r:id="rId1"/>
     <sheet name="SourceObject" sheetId="1" r:id="rId2"/>
-    <sheet name="CopyMappings" sheetId="3" r:id="rId3"/>
+    <sheet name="CopySource" sheetId="4" r:id="rId3"/>
+    <sheet name="DataLoadingBehavior" sheetId="5" r:id="rId4"/>
+    <sheet name="Trigger" sheetId="6" r:id="rId5"/>
+    <sheet name="CopyMappings" sheetId="3" r:id="rId6"/>
+    <sheet name="CopyActivity" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>schema</t>
   </si>
@@ -100,9 +104,6 @@
     <t>04ab04b7-5f05-47c6-9f07-703406b01da6</t>
   </si>
   <si>
-    <t>Bos-Is-The-Admin</t>
-  </si>
-  <si>
     <t>AzureSQL_AdventureWorks</t>
   </si>
   <si>
@@ -125,6 +126,54 @@
   </si>
   <si>
     <t>Activity</t>
+  </si>
+  <si>
+    <t>partitionOption</t>
+  </si>
+  <si>
+    <t>sqlReaderQuery</t>
+  </si>
+  <si>
+    <t>partitionLowerBound</t>
+  </si>
+  <si>
+    <t>partitionUpperBound</t>
+  </si>
+  <si>
+    <t>partitionColumnName</t>
+  </si>
+  <si>
+    <t>partitionNames</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>SELECT *  FROM dbo.SalesHistory</t>
+  </si>
+  <si>
+    <t>dataLoadingBehavior</t>
+  </si>
+  <si>
+    <t>watermarkColumnName</t>
+  </si>
+  <si>
+    <t>watermarkColumnType</t>
+  </si>
+  <si>
+    <t>watermarkColumnStartValue</t>
+  </si>
+  <si>
+    <t>FullLoad</t>
+  </si>
+  <si>
+    <t>Sandbox</t>
+  </si>
+  <si>
+    <t>Trigger_SalesHistory</t>
+  </si>
+  <si>
+    <t>Bob-Is-The-Admin</t>
   </si>
 </sst>
 </file>
@@ -478,7 +527,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264C8553-1BF2-4D7E-9CC6-2B191FA668CB}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -519,10 +570,10 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
         <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
       </c>
       <c r="G2">
         <v>42</v>
@@ -537,7 +588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881799B7-AE6F-4EC0-858E-CF4C37A4E3DE}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -563,10 +616,112 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A785076-E021-4C77-8EA7-4B290F554D9C}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8E1CAA-0540-415E-A94C-6E82BF3E921D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD7920F-77F3-46C6-9E2C-74420A0E12BB}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D06F03D-35A1-4851-B6B3-85B36F087F9B}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="A1:C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -589,86 +744,165 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DD69B0-3F06-45F1-B6E2-C1841150F0FA}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>